<commit_message>
Adding excel calculatios spreadsheet
</commit_message>
<xml_diff>
--- a/enunciado/Listado equipos.xlsx
+++ b/enunciado/Listado equipos.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camel\Google Drive\Curso Vapor\Proyecto Final\Nutricion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Documents\JAIME\Sistemas de Vapor\TrabajoFinal\Pvapor\enunciado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4178A-A80C-4263-9C1E-E77EEDDF1F25}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224ADA54-4B20-4BC2-BE87-60CBA09D0CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="480" yWindow="90" windowWidth="15480" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Previstas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Previstas!$A$13:$AB$194</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Previstas!$A$1:$AB$195</definedName>
     <definedName name="BuiltIn_AutoFilter___1">#REF!</definedName>
     <definedName name="BuiltIn_AutoFilter___1_1">#REF!</definedName>
     <definedName name="BuiltIn_AutoFilter___1_2">#REF!</definedName>
@@ -25,6 +24,7 @@
     <definedName name="BuiltIn_AutoFilter___1_4">Previstas!$A$9:$E$11</definedName>
     <definedName name="BuiltIn_AutoFilter___1_5">Previstas!$A$9:$E$11</definedName>
     <definedName name="BuiltIn_AutoFilter___1_6">Previstas!$A$9:$E$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Previstas!$A$1:$AB$195</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Previstas!$1:$11</definedName>
     <definedName name="unnamed">#REF!</definedName>
     <definedName name="unnamed_1">Previstas!$A$9:$E$9</definedName>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="432">
   <si>
     <t>ITEM</t>
   </si>
@@ -1338,6 +1338,9 @@
   </si>
   <si>
     <t>S46</t>
+  </si>
+  <si>
+    <t>SE REQUIERE ESTACION REGULACION DE VAPOR. ADEMAS EL DRENAJE DEBE DE SER CON TUBERIA PARA ALTA TEMPERATURA O (HIERRO NEGRO). CONEXIÓN REQUIERE DESCONECTADOR CON COLA DE CABLE CON BIEX DE 1,5METROS. TEMP.MAXIMA 100°C.accion directa, vallvula de regulacion de presion. MAximo psi--para las marmitas</t>
   </si>
 </sst>
 </file>
@@ -2362,10 +2365,67 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2385,15 +2445,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2421,54 +2472,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6478,7 +6481,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6801,46 +6804,46 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:GN194"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="11" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="1" tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <pane xSplit="5" ySplit="11" topLeftCell="F144" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="H91" sqref="H91"/>
+      <selection pane="bottomRight" activeCell="AA145" sqref="AA145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="42" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="8" width="5.5703125" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" customWidth="1"/>
+    <col min="7" max="8" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="4" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="3" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="3.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="4.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5546875" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="4.6640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="25" max="26" width="6.42578125" customWidth="1"/>
-    <col min="27" max="27" width="41.5703125" style="99" customWidth="1"/>
-    <col min="28" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5546875" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="6.44140625" customWidth="1"/>
+    <col min="27" max="27" width="41.5546875" style="99" customWidth="1"/>
+    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:196" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="122"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+    <row r="1" spans="1:196" s="1" customFormat="1" ht="24.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="117"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
       <c r="D1" s="14"/>
       <c r="E1" s="43"/>
       <c r="F1" s="18"/>
@@ -7035,7 +7038,7 @@
       <c r="GM1" s="2"/>
       <c r="GN1" s="2"/>
     </row>
-    <row r="2" spans="1:196" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:196" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="40"/>
@@ -7233,13 +7236,13 @@
       <c r="GM2" s="2"/>
       <c r="GN2" s="2"/>
     </row>
-    <row r="3" spans="1:196" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="102" t="s">
+    <row r="3" spans="1:196" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
       <c r="E3" s="44"/>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
@@ -7433,11 +7436,11 @@
       <c r="GM3" s="2"/>
       <c r="GN3" s="2"/>
     </row>
-    <row r="4" spans="1:196" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="102"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
+    <row r="4" spans="1:196" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="119"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
       <c r="E4" s="44"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
@@ -7631,13 +7634,13 @@
       <c r="GM4" s="2"/>
       <c r="GN4" s="2"/>
     </row>
-    <row r="5" spans="1:196" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="102" t="s">
+    <row r="5" spans="1:196" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
       <c r="E5" s="44"/>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
@@ -7831,13 +7834,13 @@
       <c r="GM5" s="2"/>
       <c r="GN5" s="2"/>
     </row>
-    <row r="6" spans="1:196" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="124" t="s">
+    <row r="6" spans="1:196" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="125"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
       <c r="E6" s="44"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -8031,11 +8034,11 @@
       <c r="GM6" s="2"/>
       <c r="GN6" s="2"/>
     </row>
-    <row r="7" spans="1:196" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
+    <row r="7" spans="1:196" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="119"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
       <c r="E7" s="44"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -8229,11 +8232,11 @@
       <c r="GM7" s="2"/>
       <c r="GN7" s="2"/>
     </row>
-    <row r="8" spans="1:196" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
+    <row r="8" spans="1:196" s="1" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="119"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
       <c r="E8" s="44"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -8427,47 +8430,47 @@
       <c r="GM8" s="2"/>
       <c r="GN8" s="2"/>
     </row>
-    <row r="9" spans="1:196" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129" t="s">
+    <row r="9" spans="1:196" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="132" t="s">
+      <c r="B9" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C9" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="116" t="s">
+      <c r="E9" s="132" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119"/>
-      <c r="T9" s="119"/>
-      <c r="U9" s="119"/>
-      <c r="V9" s="119"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="135"/>
+      <c r="L9" s="135"/>
+      <c r="M9" s="135"/>
+      <c r="N9" s="135"/>
+      <c r="O9" s="135"/>
+      <c r="P9" s="135"/>
+      <c r="Q9" s="135"/>
+      <c r="R9" s="135"/>
+      <c r="S9" s="135"/>
+      <c r="T9" s="135"/>
+      <c r="U9" s="135"/>
+      <c r="V9" s="135"/>
       <c r="W9" s="91"/>
       <c r="X9" s="91"/>
       <c r="Y9" s="46"/>
       <c r="Z9" s="46"/>
-      <c r="AA9" s="107" t="s">
+      <c r="AA9" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="AB9" s="126" t="s">
+      <c r="AB9" s="102" t="s">
         <v>0</v>
       </c>
       <c r="AC9" s="2"/>
@@ -8639,47 +8642,47 @@
       <c r="GM9" s="2"/>
       <c r="GN9" s="2"/>
     </row>
-    <row r="10" spans="1:196" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
-      <c r="B10" s="133"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="110" t="s">
+    <row r="10" spans="1:196" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="109"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="111"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="110" t="s">
+      <c r="G10" s="106"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="111"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="110" t="s">
+      <c r="J10" s="106"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="111"/>
-      <c r="N10" s="111"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="111"/>
-      <c r="Q10" s="111"/>
-      <c r="R10" s="111"/>
-      <c r="S10" s="111"/>
-      <c r="T10" s="110" t="s">
+      <c r="M10" s="106"/>
+      <c r="N10" s="106"/>
+      <c r="O10" s="106"/>
+      <c r="P10" s="106"/>
+      <c r="Q10" s="106"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="106"/>
+      <c r="T10" s="105" t="s">
         <v>419</v>
       </c>
-      <c r="U10" s="111"/>
-      <c r="V10" s="111"/>
-      <c r="W10" s="120" t="s">
+      <c r="U10" s="106"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="X10" s="121"/>
-      <c r="Y10" s="110" t="s">
+      <c r="X10" s="137"/>
+      <c r="Y10" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="Z10" s="111"/>
-      <c r="AA10" s="108"/>
-      <c r="AB10" s="127"/>
+      <c r="Z10" s="106"/>
+      <c r="AA10" s="127"/>
+      <c r="AB10" s="103"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
@@ -8849,12 +8852,12 @@
       <c r="GM10" s="2"/>
       <c r="GN10" s="2"/>
     </row>
-    <row r="11" spans="1:196" s="12" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="131"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="118"/>
+    <row r="11" spans="1:196" s="12" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="110"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="134"/>
       <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
@@ -8918,8 +8921,8 @@
       <c r="Z11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AA11" s="109"/>
-      <c r="AB11" s="128"/>
+      <c r="AA11" s="128"/>
+      <c r="AB11" s="104"/>
       <c r="AC11" s="11"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="11"/>
@@ -9089,12 +9092,12 @@
       <c r="GM11" s="11"/>
       <c r="GN11" s="11"/>
     </row>
-    <row r="12" spans="1:196" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="104" t="s">
+    <row r="12" spans="1:196" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="105"/>
-      <c r="C12" s="106"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
       <c r="F12" s="31"/>
@@ -9121,7 +9124,7 @@
       <c r="AA12" s="93"/>
       <c r="AB12" s="47"/>
     </row>
-    <row r="13" spans="1:196" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:196" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="41"/>
@@ -9151,7 +9154,7 @@
       <c r="AA13" s="94"/>
       <c r="AB13" s="10"/>
     </row>
-    <row r="14" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>41</v>
       </c>
@@ -9193,7 +9196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="72"/>
       <c r="B15" s="73"/>
       <c r="C15" s="74"/>
@@ -9223,7 +9226,7 @@
       <c r="AA15" s="96"/>
       <c r="AB15" s="72"/>
     </row>
-    <row r="16" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:196" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>35</v>
       </c>
@@ -9265,7 +9268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="72"/>
       <c r="B17" s="73"/>
       <c r="C17" s="74"/>
@@ -9295,7 +9298,7 @@
       <c r="AA17" s="96"/>
       <c r="AB17" s="72"/>
     </row>
-    <row r="18" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>40</v>
       </c>
@@ -9337,7 +9340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
       <c r="B19" s="73"/>
       <c r="C19" s="74"/>
@@ -9367,7 +9370,7 @@
       <c r="AA19" s="96"/>
       <c r="AB19" s="72"/>
     </row>
-    <row r="20" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>47</v>
       </c>
@@ -9421,7 +9424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
       <c r="B21" s="73"/>
       <c r="C21" s="74"/>
@@ -9451,7 +9454,7 @@
       <c r="AA21" s="96"/>
       <c r="AB21" s="72"/>
     </row>
-    <row r="22" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>45</v>
       </c>
@@ -9503,7 +9506,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>45</v>
       </c>
@@ -9545,7 +9548,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="72"/>
       <c r="B24" s="73"/>
       <c r="C24" s="74"/>
@@ -9575,7 +9578,7 @@
       <c r="AA24" s="96"/>
       <c r="AB24" s="72"/>
     </row>
-    <row r="25" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>52</v>
       </c>
@@ -9627,7 +9630,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="72"/>
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
@@ -9657,7 +9660,7 @@
       <c r="AA26" s="96"/>
       <c r="AB26" s="72"/>
     </row>
-    <row r="27" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>57</v>
       </c>
@@ -9699,7 +9702,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
       <c r="B28" s="73"/>
       <c r="C28" s="74"/>
@@ -9729,7 +9732,7 @@
       <c r="AA28" s="96"/>
       <c r="AB28" s="72"/>
     </row>
-    <row r="29" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>63</v>
       </c>
@@ -9791,7 +9794,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="72"/>
       <c r="B30" s="73"/>
       <c r="C30" s="74"/>
@@ -9821,7 +9824,7 @@
       <c r="AA30" s="96"/>
       <c r="AB30" s="72"/>
     </row>
-    <row r="31" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
         <v>48</v>
       </c>
@@ -9875,7 +9878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="72"/>
       <c r="B32" s="73"/>
       <c r="C32" s="74"/>
@@ -9905,7 +9908,7 @@
       <c r="AA32" s="96"/>
       <c r="AB32" s="72"/>
     </row>
-    <row r="33" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>304</v>
       </c>
@@ -9959,7 +9962,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
         <v>303</v>
       </c>
@@ -10001,7 +10004,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="72"/>
       <c r="B35" s="73"/>
       <c r="C35" s="74"/>
@@ -10031,7 +10034,7 @@
       <c r="AA35" s="96"/>
       <c r="AB35" s="72"/>
     </row>
-    <row r="36" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>51</v>
       </c>
@@ -10083,7 +10086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="72"/>
       <c r="B37" s="73"/>
       <c r="C37" s="74"/>
@@ -10113,7 +10116,7 @@
       <c r="AA37" s="96"/>
       <c r="AB37" s="72"/>
     </row>
-    <row r="38" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
         <v>306</v>
       </c>
@@ -10155,7 +10158,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
         <v>60</v>
       </c>
@@ -10209,7 +10212,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
         <v>301</v>
       </c>
@@ -10251,7 +10254,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="72"/>
       <c r="B41" s="73"/>
       <c r="C41" s="74"/>
@@ -10281,7 +10284,7 @@
       <c r="AA41" s="96"/>
       <c r="AB41" s="72"/>
     </row>
-    <row r="42" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
         <v>69</v>
       </c>
@@ -10335,7 +10338,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="72"/>
       <c r="B43" s="73"/>
       <c r="C43" s="74"/>
@@ -10365,7 +10368,7 @@
       <c r="AA43" s="96"/>
       <c r="AB43" s="72"/>
     </row>
-    <row r="44" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
         <v>65</v>
       </c>
@@ -10417,7 +10420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="72"/>
       <c r="B45" s="73"/>
       <c r="C45" s="74"/>
@@ -10447,7 +10450,7 @@
       <c r="AA45" s="96"/>
       <c r="AB45" s="72"/>
     </row>
-    <row r="46" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
         <v>39</v>
       </c>
@@ -10501,7 +10504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="72"/>
       <c r="B47" s="73"/>
       <c r="C47" s="74"/>
@@ -10531,7 +10534,7 @@
       <c r="AA47" s="96"/>
       <c r="AB47" s="72"/>
     </row>
-    <row r="48" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
         <v>56</v>
       </c>
@@ -10583,7 +10586,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="72"/>
       <c r="B49" s="73"/>
       <c r="C49" s="74"/>
@@ -10613,7 +10616,7 @@
       <c r="AA49" s="96"/>
       <c r="AB49" s="72"/>
     </row>
-    <row r="50" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
         <v>44</v>
       </c>
@@ -10665,7 +10668,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="72"/>
       <c r="B51" s="73"/>
       <c r="C51" s="74"/>
@@ -10695,7 +10698,7 @@
       <c r="AA51" s="96"/>
       <c r="AB51" s="72"/>
     </row>
-    <row r="52" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>67</v>
       </c>
@@ -10749,7 +10752,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="72"/>
       <c r="B53" s="73"/>
       <c r="C53" s="74"/>
@@ -10779,7 +10782,7 @@
       <c r="AA53" s="96"/>
       <c r="AB53" s="72"/>
     </row>
-    <row r="54" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
         <v>73</v>
       </c>
@@ -10825,7 +10828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
         <v>74</v>
       </c>
@@ -10871,7 +10874,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="72"/>
       <c r="B56" s="73"/>
       <c r="C56" s="74"/>
@@ -10901,7 +10904,7 @@
       <c r="AA56" s="96"/>
       <c r="AB56" s="72"/>
     </row>
-    <row r="57" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
         <v>310</v>
       </c>
@@ -10953,7 +10956,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
         <v>311</v>
       </c>
@@ -10995,7 +10998,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="72"/>
       <c r="B59" s="73"/>
       <c r="C59" s="74"/>
@@ -11025,7 +11028,7 @@
       <c r="AA59" s="96"/>
       <c r="AB59" s="72"/>
     </row>
-    <row r="60" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
         <v>58</v>
       </c>
@@ -11067,7 +11070,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="72"/>
       <c r="B61" s="73"/>
       <c r="C61" s="74"/>
@@ -11097,7 +11100,7 @@
       <c r="AA61" s="96"/>
       <c r="AB61" s="72"/>
     </row>
-    <row r="62" spans="1:28" s="87" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="87" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
         <v>76</v>
       </c>
@@ -11147,7 +11150,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="72"/>
       <c r="B63" s="73"/>
       <c r="C63" s="74"/>
@@ -11177,7 +11180,7 @@
       <c r="AA63" s="96"/>
       <c r="AB63" s="72"/>
     </row>
-    <row r="64" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="69" t="s">
         <v>237</v>
       </c>
@@ -11227,7 +11230,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="72"/>
       <c r="B65" s="73"/>
       <c r="C65" s="74"/>
@@ -11257,7 +11260,7 @@
       <c r="AA65" s="96"/>
       <c r="AB65" s="72"/>
     </row>
-    <row r="66" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
         <v>87</v>
       </c>
@@ -11307,7 +11310,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="72"/>
       <c r="B67" s="73"/>
       <c r="C67" s="74"/>
@@ -11337,7 +11340,7 @@
       <c r="AA67" s="96"/>
       <c r="AB67" s="72"/>
     </row>
-    <row r="68" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
         <v>91</v>
       </c>
@@ -11387,7 +11390,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="72"/>
       <c r="B69" s="73"/>
       <c r="C69" s="74"/>
@@ -11417,7 +11420,7 @@
       <c r="AA69" s="96"/>
       <c r="AB69" s="72"/>
     </row>
-    <row r="70" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
         <v>108</v>
       </c>
@@ -11467,7 +11470,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="72"/>
       <c r="B71" s="73"/>
       <c r="C71" s="74"/>
@@ -11497,7 +11500,7 @@
       <c r="AA71" s="96"/>
       <c r="AB71" s="72"/>
     </row>
-    <row r="72" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
         <v>163</v>
       </c>
@@ -11547,7 +11550,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="72"/>
       <c r="B73" s="73"/>
       <c r="C73" s="74"/>
@@ -11577,7 +11580,7 @@
       <c r="AA73" s="96"/>
       <c r="AB73" s="72"/>
     </row>
-    <row r="74" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="69" t="s">
         <v>266</v>
       </c>
@@ -11631,7 +11634,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
         <v>247</v>
       </c>
@@ -11683,7 +11686,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
         <v>255</v>
       </c>
@@ -11725,7 +11728,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
         <v>262</v>
       </c>
@@ -11767,7 +11770,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="72"/>
       <c r="B78" s="73"/>
       <c r="C78" s="74"/>
@@ -11797,7 +11800,7 @@
       <c r="AA78" s="96"/>
       <c r="AB78" s="72"/>
     </row>
-    <row r="79" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
         <v>214</v>
       </c>
@@ -11839,7 +11842,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
         <v>215</v>
       </c>
@@ -11891,7 +11894,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
         <v>216</v>
       </c>
@@ -11933,7 +11936,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="48" t="s">
         <v>213</v>
       </c>
@@ -11985,7 +11988,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
         <v>202</v>
       </c>
@@ -12027,7 +12030,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
         <v>201</v>
       </c>
@@ -12069,7 +12072,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
         <v>199</v>
       </c>
@@ -12115,7 +12118,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="72"/>
       <c r="B86" s="73"/>
       <c r="C86" s="74"/>
@@ -12145,7 +12148,7 @@
       <c r="AA86" s="96"/>
       <c r="AB86" s="72"/>
     </row>
-    <row r="87" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
         <v>81</v>
       </c>
@@ -12199,7 +12202,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
         <v>230</v>
       </c>
@@ -12253,7 +12256,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
         <v>231</v>
       </c>
@@ -12307,7 +12310,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="72"/>
       <c r="B90" s="73"/>
       <c r="C90" s="74"/>
@@ -12337,7 +12340,7 @@
       <c r="AA90" s="96"/>
       <c r="AB90" s="72"/>
     </row>
-    <row r="91" spans="1:28" s="59" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" s="59" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
         <v>426</v>
       </c>
@@ -12385,7 +12388,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="92" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="72"/>
       <c r="B92" s="73"/>
       <c r="C92" s="74"/>
@@ -12415,7 +12418,7 @@
       <c r="AA92" s="96"/>
       <c r="AB92" s="72"/>
     </row>
-    <row r="93" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="48" t="s">
         <v>240</v>
       </c>
@@ -12469,7 +12472,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="94" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="72"/>
       <c r="B94" s="73"/>
       <c r="C94" s="74"/>
@@ -12499,7 +12502,7 @@
       <c r="AA94" s="96"/>
       <c r="AB94" s="72"/>
     </row>
-    <row r="95" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="48" t="s">
         <v>244</v>
       </c>
@@ -12553,7 +12556,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="96" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="72"/>
       <c r="B96" s="73"/>
       <c r="C96" s="74"/>
@@ -12583,7 +12586,7 @@
       <c r="AA96" s="96"/>
       <c r="AB96" s="72"/>
     </row>
-    <row r="97" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="48" t="s">
         <v>263</v>
       </c>
@@ -12637,7 +12640,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="98" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="72"/>
       <c r="B98" s="73"/>
       <c r="C98" s="74"/>
@@ -12667,7 +12670,7 @@
       <c r="AA98" s="96"/>
       <c r="AB98" s="72"/>
     </row>
-    <row r="99" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="48" t="s">
         <v>256</v>
       </c>
@@ -12723,7 +12726,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="100" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="48"/>
       <c r="B100" s="49" t="s">
         <v>241</v>
@@ -12775,7 +12778,7 @@
       </c>
       <c r="AB100" s="48"/>
     </row>
-    <row r="101" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="72"/>
       <c r="B101" s="73"/>
       <c r="C101" s="74"/>
@@ -12805,7 +12808,7 @@
       <c r="AA101" s="96"/>
       <c r="AB101" s="72"/>
     </row>
-    <row r="102" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="48" t="s">
         <v>80</v>
       </c>
@@ -12859,7 +12862,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="72"/>
       <c r="B103" s="73"/>
       <c r="C103" s="74"/>
@@ -12889,7 +12892,7 @@
       <c r="AA103" s="96"/>
       <c r="AB103" s="72"/>
     </row>
-    <row r="104" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="48" t="s">
         <v>192</v>
       </c>
@@ -12931,7 +12934,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="105" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="72"/>
       <c r="B105" s="73"/>
       <c r="C105" s="74"/>
@@ -12961,7 +12964,7 @@
       <c r="AA105" s="96"/>
       <c r="AB105" s="72"/>
     </row>
-    <row r="106" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="48" t="s">
         <v>224</v>
       </c>
@@ -13003,7 +13006,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="107" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="72"/>
       <c r="B107" s="73"/>
       <c r="C107" s="74"/>
@@ -13033,7 +13036,7 @@
       <c r="AA107" s="96"/>
       <c r="AB107" s="72"/>
     </row>
-    <row r="108" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="48" t="s">
         <v>166</v>
       </c>
@@ -13075,7 +13078,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="109" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="72"/>
       <c r="B109" s="73"/>
       <c r="C109" s="74"/>
@@ -13105,7 +13108,7 @@
       <c r="AA109" s="96"/>
       <c r="AB109" s="72"/>
     </row>
-    <row r="110" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="48" t="s">
         <v>160</v>
       </c>
@@ -13147,7 +13150,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="72"/>
       <c r="B111" s="73"/>
       <c r="C111" s="74"/>
@@ -13177,7 +13180,7 @@
       <c r="AA111" s="96"/>
       <c r="AB111" s="72"/>
     </row>
-    <row r="112" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="48" t="s">
         <v>102</v>
       </c>
@@ -13219,7 +13222,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="72"/>
       <c r="B113" s="73"/>
       <c r="C113" s="74"/>
@@ -13249,7 +13252,7 @@
       <c r="AA113" s="96"/>
       <c r="AB113" s="72"/>
     </row>
-    <row r="114" spans="1:28" s="68" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:28" s="68" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="48" t="s">
         <v>390</v>
       </c>
@@ -13291,7 +13294,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="72"/>
       <c r="B115" s="73"/>
       <c r="C115" s="74"/>
@@ -13321,7 +13324,7 @@
       <c r="AA115" s="96"/>
       <c r="AB115" s="72"/>
     </row>
-    <row r="116" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="48" t="s">
         <v>151</v>
       </c>
@@ -13363,7 +13366,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="117" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="72"/>
       <c r="B117" s="73"/>
       <c r="C117" s="74"/>
@@ -13393,7 +13396,7 @@
       <c r="AA117" s="96"/>
       <c r="AB117" s="72"/>
     </row>
-    <row r="118" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="48" t="s">
         <v>227</v>
       </c>
@@ -13447,7 +13450,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="119" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="72"/>
       <c r="B119" s="73"/>
       <c r="C119" s="74"/>
@@ -13477,7 +13480,7 @@
       <c r="AA119" s="96"/>
       <c r="AB119" s="72"/>
     </row>
-    <row r="120" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="48" t="s">
         <v>185</v>
       </c>
@@ -13531,7 +13534,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="72"/>
       <c r="B121" s="73"/>
       <c r="C121" s="74"/>
@@ -13561,7 +13564,7 @@
       <c r="AA121" s="96"/>
       <c r="AB121" s="72"/>
     </row>
-    <row r="122" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="48" t="s">
         <v>259</v>
       </c>
@@ -13603,7 +13606,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="123" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="72"/>
       <c r="B123" s="73"/>
       <c r="C123" s="74"/>
@@ -13633,7 +13636,7 @@
       <c r="AA123" s="96"/>
       <c r="AB123" s="72"/>
     </row>
-    <row r="124" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="48" t="s">
         <v>251</v>
       </c>
@@ -13685,7 +13688,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="72"/>
       <c r="B125" s="73"/>
       <c r="C125" s="74"/>
@@ -13715,7 +13718,7 @@
       <c r="AA125" s="96"/>
       <c r="AB125" s="72"/>
     </row>
-    <row r="126" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="48" t="s">
         <v>125</v>
       </c>
@@ -13769,7 +13772,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="48" t="s">
         <v>125</v>
       </c>
@@ -13823,7 +13826,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="72"/>
       <c r="B128" s="73"/>
       <c r="C128" s="74"/>
@@ -13853,7 +13856,7 @@
       <c r="AA128" s="96"/>
       <c r="AB128" s="72"/>
     </row>
-    <row r="129" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="48" t="s">
         <v>106</v>
       </c>
@@ -13905,7 +13908,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="130" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="72"/>
       <c r="B130" s="73"/>
       <c r="C130" s="74"/>
@@ -13935,7 +13938,7 @@
       <c r="AA130" s="96"/>
       <c r="AB130" s="72"/>
     </row>
-    <row r="131" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="48" t="s">
         <v>107</v>
       </c>
@@ -13987,7 +13990,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="132" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="72"/>
       <c r="B132" s="73"/>
       <c r="C132" s="74"/>
@@ -14017,7 +14020,7 @@
       <c r="AA132" s="96"/>
       <c r="AB132" s="72"/>
     </row>
-    <row r="133" spans="1:28" s="59" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:28" s="59" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A133" s="48" t="s">
         <v>425</v>
       </c>
@@ -14091,7 +14094,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="134" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="48" t="s">
         <v>401</v>
       </c>
@@ -14147,7 +14150,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="135" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="48" t="s">
         <v>402</v>
       </c>
@@ -14201,7 +14204,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="136" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="48" t="s">
         <v>156</v>
       </c>
@@ -14255,7 +14258,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="48" t="s">
         <v>156</v>
       </c>
@@ -14297,7 +14300,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="138" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="48" t="s">
         <v>157</v>
       </c>
@@ -14339,7 +14342,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="139" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="72"/>
       <c r="B139" s="73"/>
       <c r="C139" s="74"/>
@@ -14369,7 +14372,7 @@
       <c r="AA139" s="96"/>
       <c r="AB139" s="72"/>
     </row>
-    <row r="140" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="48" t="s">
         <v>117</v>
       </c>
@@ -14431,7 +14434,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="48" t="s">
         <v>117</v>
       </c>
@@ -14481,7 +14484,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="48" t="s">
         <v>118</v>
       </c>
@@ -14535,7 +14538,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="143" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="48" t="s">
         <v>119</v>
       </c>
@@ -14577,7 +14580,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="72"/>
       <c r="B144" s="73"/>
       <c r="C144" s="74"/>
@@ -14607,7 +14610,7 @@
       <c r="AA144" s="96"/>
       <c r="AB144" s="72"/>
     </row>
-    <row r="145" spans="1:28" s="59" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:28" s="59" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A145" s="48" t="s">
         <v>427</v>
       </c>
@@ -14675,13 +14678,13 @@
         <v>410</v>
       </c>
       <c r="AA145" s="98" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="AB145" s="48" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="48" t="s">
         <v>403</v>
       </c>
@@ -14737,7 +14740,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="1:28" s="67" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:28" s="67" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="48" t="s">
         <v>404</v>
       </c>
@@ -14787,7 +14790,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="48" t="s">
         <v>196</v>
       </c>
@@ -14841,7 +14844,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="149" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="48" t="s">
         <v>197</v>
       </c>
@@ -14883,7 +14886,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="150" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="72"/>
       <c r="B150" s="73"/>
       <c r="C150" s="74"/>
@@ -14913,7 +14916,7 @@
       <c r="AA150" s="96"/>
       <c r="AB150" s="72"/>
     </row>
-    <row r="151" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="48" t="s">
         <v>200</v>
       </c>
@@ -14975,7 +14978,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="72"/>
       <c r="B152" s="73"/>
       <c r="C152" s="74"/>
@@ -15005,7 +15008,7 @@
       <c r="AA152" s="96"/>
       <c r="AB152" s="72"/>
     </row>
-    <row r="153" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="48" t="s">
         <v>184</v>
       </c>
@@ -15065,7 +15068,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="154" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="48" t="s">
         <v>184</v>
       </c>
@@ -15115,7 +15118,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="155" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="72"/>
       <c r="B155" s="73"/>
       <c r="C155" s="74"/>
@@ -15145,7 +15148,7 @@
       <c r="AA155" s="96"/>
       <c r="AB155" s="72"/>
     </row>
-    <row r="156" spans="1:28" s="59" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:28" s="59" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A156" s="48" t="s">
         <v>429</v>
       </c>
@@ -15209,7 +15212,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="157" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="72"/>
       <c r="B157" s="73"/>
       <c r="C157" s="74"/>
@@ -15239,7 +15242,7 @@
       <c r="AA157" s="96"/>
       <c r="AB157" s="72"/>
     </row>
-    <row r="158" spans="1:28" s="59" customFormat="1" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:28" s="59" customFormat="1" ht="105.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="48" t="s">
         <v>236</v>
       </c>
@@ -15301,7 +15304,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="159" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="72"/>
       <c r="B159" s="73"/>
       <c r="C159" s="74"/>
@@ -15331,7 +15334,7 @@
       <c r="AA159" s="96"/>
       <c r="AB159" s="72"/>
     </row>
-    <row r="160" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="48" t="s">
         <v>405</v>
       </c>
@@ -15393,7 +15396,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="161" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="48" t="s">
         <v>406</v>
       </c>
@@ -15451,7 +15454,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="162" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="72"/>
       <c r="B162" s="73"/>
       <c r="C162" s="74"/>
@@ -15481,7 +15484,7 @@
       <c r="AA162" s="96"/>
       <c r="AB162" s="72"/>
     </row>
-    <row r="163" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="48" t="s">
         <v>98</v>
       </c>
@@ -15523,7 +15526,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="164" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="72"/>
       <c r="B164" s="73"/>
       <c r="C164" s="74"/>
@@ -15553,7 +15556,7 @@
       <c r="AA164" s="96"/>
       <c r="AB164" s="72"/>
     </row>
-    <row r="165" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="48" t="s">
         <v>132</v>
       </c>
@@ -15603,7 +15606,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="166" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="72"/>
       <c r="B166" s="73"/>
       <c r="C166" s="74"/>
@@ -15633,7 +15636,7 @@
       <c r="AA166" s="96"/>
       <c r="AB166" s="72"/>
     </row>
-    <row r="167" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="48" t="s">
         <v>136</v>
       </c>
@@ -15685,7 +15688,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="168" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="72"/>
       <c r="B168" s="73"/>
       <c r="C168" s="74"/>
@@ -15715,7 +15718,7 @@
       <c r="AA168" s="96"/>
       <c r="AB168" s="72"/>
     </row>
-    <row r="169" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="48" t="s">
         <v>129</v>
       </c>
@@ -15769,7 +15772,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="170" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="72"/>
       <c r="B170" s="73"/>
       <c r="C170" s="74"/>
@@ -15799,7 +15802,7 @@
       <c r="AA170" s="96"/>
       <c r="AB170" s="72"/>
     </row>
-    <row r="171" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="48" t="s">
         <v>94</v>
       </c>
@@ -15851,7 +15854,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="172" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:28" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="72"/>
       <c r="B172" s="73"/>
       <c r="C172" s="74"/>
@@ -15881,7 +15884,7 @@
       <c r="AA172" s="96"/>
       <c r="AB172" s="72"/>
     </row>
-    <row r="173" spans="1:28" s="59" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:28" s="59" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A173" s="48" t="s">
         <v>430</v>
       </c>
@@ -15947,7 +15950,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="72"/>
       <c r="B174" s="73"/>
       <c r="C174" s="74"/>
@@ -15977,7 +15980,7 @@
       <c r="AA174" s="96"/>
       <c r="AB174" s="72"/>
     </row>
-    <row r="175" spans="1:28" s="59" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:28" s="59" customFormat="1" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="48" t="s">
         <v>144</v>
       </c>
@@ -16031,7 +16034,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="176" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="72"/>
       <c r="B176" s="73"/>
       <c r="C176" s="74"/>
@@ -16061,7 +16064,7 @@
       <c r="AA176" s="96"/>
       <c r="AB176" s="72"/>
     </row>
-    <row r="177" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="48" t="s">
         <v>171</v>
       </c>
@@ -16109,7 +16112,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="178" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="48" t="s">
         <v>170</v>
       </c>
@@ -16157,7 +16160,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="72"/>
       <c r="B179" s="73"/>
       <c r="C179" s="74"/>
@@ -16187,7 +16190,7 @@
       <c r="AA179" s="96"/>
       <c r="AB179" s="72"/>
     </row>
-    <row r="180" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="48" t="s">
         <v>288</v>
       </c>
@@ -16241,7 +16244,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="181" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="72"/>
       <c r="B181" s="73"/>
       <c r="C181" s="74"/>
@@ -16271,7 +16274,7 @@
       <c r="AA181" s="96"/>
       <c r="AB181" s="72"/>
     </row>
-    <row r="182" spans="1:28" s="59" customFormat="1" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:28" s="59" customFormat="1" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="48" t="s">
         <v>391</v>
       </c>
@@ -16341,7 +16344,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="183" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="72"/>
       <c r="B183" s="73"/>
       <c r="C183" s="74"/>
@@ -16371,7 +16374,7 @@
       <c r="AA183" s="96"/>
       <c r="AB183" s="72"/>
     </row>
-    <row r="184" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:28" s="59" customFormat="1" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="48" t="s">
         <v>392</v>
       </c>
@@ -16423,7 +16426,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="185" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="72"/>
       <c r="B185" s="73"/>
       <c r="C185" s="74"/>
@@ -16453,7 +16456,7 @@
       <c r="AA185" s="96"/>
       <c r="AB185" s="72"/>
     </row>
-    <row r="186" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="48" t="s">
         <v>282</v>
       </c>
@@ -16503,7 +16506,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="187" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="72"/>
       <c r="B187" s="73"/>
       <c r="C187" s="74"/>
@@ -16533,7 +16536,7 @@
       <c r="AA187" s="96"/>
       <c r="AB187" s="72"/>
     </row>
-    <row r="188" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="48" t="s">
         <v>284</v>
       </c>
@@ -16575,7 +16578,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="189" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="72"/>
       <c r="B189" s="73"/>
       <c r="C189" s="74"/>
@@ -16605,7 +16608,7 @@
       <c r="AA189" s="96"/>
       <c r="AB189" s="72"/>
     </row>
-    <row r="190" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="48" t="s">
         <v>278</v>
       </c>
@@ -16655,7 +16658,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="191" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:28" s="59" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="72"/>
       <c r="B191" s="73"/>
       <c r="C191" s="74"/>
@@ -16685,7 +16688,7 @@
       <c r="AA191" s="96"/>
       <c r="AB191" s="72"/>
     </row>
-    <row r="192" spans="1:28" s="59" customFormat="1" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:28" s="59" customFormat="1" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="48" t="s">
         <v>268</v>
       </c>
@@ -16735,7 +16738,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="193" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="22"/>
       <c r="B193" s="23"/>
       <c r="C193" s="41"/>
@@ -16765,7 +16768,7 @@
       <c r="AA193" s="94"/>
       <c r="AB193" s="22"/>
     </row>
-    <row r="194" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
       <c r="B194" s="23"/>
       <c r="C194" s="41"/>
@@ -16798,19 +16801,6 @@
   </sheetData>
   <autoFilter ref="A13:AB194" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="22">
-    <mergeCell ref="AB9:AB11"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="AA9:AA11"/>
@@ -16820,6 +16810,19 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="I9:V9"/>
     <mergeCell ref="W10:X10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="AB9:AB11"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>